<commit_message>
Add support for float numbers
</commit_message>
<xml_diff>
--- a/spec/fixtures/simple_values.xlsx
+++ b/spec/fixtures/simple_values.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/Workspace/ruby-sheet/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F81CA-2A35-644A-B2EE-318285EBC73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE9D1EA-16DD-0744-A0DD-D34761444A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{94BA95AE-DB14-DA4A-AB72-BB7C5880B0F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -466,13 +466,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C17891-7691-5144-B2F6-6D3583E8DADD}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1">
@@ -531,6 +535,27 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5566778899</v>
+      </c>
+      <c r="B5">
+        <v>3.1415899999999999</v>
+      </c>
+      <c r="C5">
+        <f>A5-B5</f>
+        <v>5566778895.8584099</v>
+      </c>
+      <c r="D5">
+        <v>-33.4</v>
+      </c>
+      <c r="E5">
+        <v>-5</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>